<commit_message>
renamed excel sheet column
- `attribute_found_in_any_sheets` ==> `attribute_found_in_any_sheet` to be consistent with files circulated previously
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_template.xlsx
+++ b/inst/extdata/scidb_metadata_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/reveal-genomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5F3462-1148-0D4C-ADBD-2F4DA75D804A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E81F64-4DEC-184F-85CB-5CD76AABEE59}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="15540" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="30160" windowHeight="17700" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="1" r:id="rId1"/>
@@ -453,9 +453,6 @@
     <t>importance</t>
   </si>
   <si>
-    <t>attribute_found_in_any_sheets</t>
-  </si>
-  <si>
     <t>attribute_in_Studies</t>
   </si>
   <si>
@@ -586,6 +583,9 @@
   </si>
   <si>
     <t>data-admin needs to fill description of filters used e.g. "non-synonymous; depth &gt; XX; ..."</t>
+  </si>
+  <si>
+    <t>attribute_found_in_any_sheet</t>
   </si>
 </sst>
 </file>
@@ -2341,7 +2341,7 @@
         <v>33</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2631,13 +2631,13 @@
         <v>41</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>100</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>79</v>
@@ -2669,13 +2669,13 @@
         <v>42</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>100</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I3" s="17" t="s">
         <v>79</v>
@@ -2707,13 +2707,13 @@
         <v>43</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>102</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>79</v>
@@ -2745,13 +2745,13 @@
         <v>82</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>102</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I5" s="17" t="s">
         <v>79</v>
@@ -2880,7 +2880,7 @@
         <v>64</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>65</v>
@@ -2934,7 +2934,7 @@
         <v>60</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>62</v>
@@ -2952,16 +2952,16 @@
         <v>64</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D6" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>128</v>
-      </c>
       <c r="F6" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>63</v>
@@ -2976,16 +2976,16 @@
         <v>64</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>128</v>
-      </c>
       <c r="F7" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>63</v>
@@ -3000,16 +3000,16 @@
         <v>64</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>128</v>
-      </c>
       <c r="F8" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>63</v>
@@ -3024,16 +3024,16 @@
         <v>64</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>128</v>
-      </c>
       <c r="F9" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>63</v>
@@ -3054,7 +3054,7 @@
         <v>67</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>67</v>
@@ -3262,10 +3262,10 @@
         <v>45</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>64</v>
@@ -3280,10 +3280,10 @@
         <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>64</v>
@@ -3295,10 +3295,10 @@
         <v>Protein-Raw intensity</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>66</v>
@@ -3310,10 +3310,10 @@
         <v>Protein-LFQ</v>
       </c>
       <c r="B13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>66</v>
@@ -3345,91 +3345,91 @@
   <sheetData>
     <row r="1" spans="1:7" s="11" customFormat="1" ht="19">
       <c r="A1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
         <v>141</v>
-      </c>
-      <c r="B2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" t="s">
-        <v>142</v>
       </c>
       <c r="D2" s="26">
         <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
         <v>144</v>
       </c>
-      <c r="B3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>146</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" t="s">
         <v>147</v>
-      </c>
-      <c r="B4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" t="s">
-        <v>148</v>
       </c>
       <c r="D4" s="26">
         <v>38</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
         <v>149</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>150</v>
-      </c>
-      <c r="C5" t="s">
-        <v>151</v>
       </c>
       <c r="D5" s="26">
         <v>38</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3445,7 +3445,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18"/>
@@ -3460,7 +3460,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="167">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="161">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
@@ -3480,19 +3480,19 @@
         <v>109</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>113</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="23" customFormat="1" ht="19">
@@ -3500,7 +3500,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" s="23">
         <v>1</v>
@@ -3531,7 +3531,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" s="23">
         <v>1</v>
@@ -3562,7 +3562,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4" s="23">
         <v>1</v>
@@ -3593,7 +3593,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F5" s="23">
         <v>1</v>
@@ -3624,7 +3624,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F6" s="23">
         <v>1</v>
@@ -3655,7 +3655,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F7" s="23">
         <v>1</v>
@@ -3686,7 +3686,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F8" s="23">
         <v>1</v>
@@ -3717,10 +3717,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>116</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>117</v>
       </c>
       <c r="F9" s="23">
         <v>1</v>
@@ -3751,7 +3751,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" s="23">
         <v>1</v>
@@ -3782,7 +3782,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11" s="23">
         <v>1</v>
@@ -3813,7 +3813,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F12" s="23">
         <v>1</v>
@@ -3844,7 +3844,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F13" s="23">
         <v>1</v>
@@ -3875,10 +3875,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F14" s="23">
         <v>1</v>
@@ -3909,7 +3909,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F15" s="23">
         <v>1</v>
@@ -3940,7 +3940,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F16" s="23">
         <v>1</v>
@@ -3971,7 +3971,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F17" s="23">
         <v>1</v>
@@ -4002,7 +4002,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F18" s="23">
         <v>1</v>
@@ -4033,7 +4033,7 @@
         <v>33</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F19" s="23">
         <v>1</v>
@@ -4061,13 +4061,13 @@
     </row>
     <row r="20" spans="1:11" s="23" customFormat="1" ht="19">
       <c r="A20" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F20" s="23">
         <v>1</v>
@@ -4098,7 +4098,7 @@
         <v>39</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F21" s="23">
         <v>1</v>
@@ -4129,7 +4129,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F22" s="23">
         <v>1</v>
@@ -4160,10 +4160,10 @@
         <v>44</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F23" s="23">
         <v>1</v>
@@ -4194,7 +4194,7 @@
         <v>47</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F24" s="23">
         <v>1</v>
@@ -4225,10 +4225,10 @@
         <v>49</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F25" s="23">
         <v>1</v>
@@ -4259,7 +4259,7 @@
         <v>69</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F26" s="23">
         <v>1</v>
@@ -4290,7 +4290,7 @@
         <v>70</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F27" s="23">
         <v>1</v>
@@ -4321,7 +4321,7 @@
         <v>71</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F28" s="23">
         <v>1</v>
@@ -4352,7 +4352,7 @@
         <v>72</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F29" s="23">
         <v>1</v>
@@ -4383,7 +4383,7 @@
         <v>73</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F30" s="23">
         <v>1</v>
@@ -4414,7 +4414,7 @@
         <v>74</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F31" s="23">
         <v>1</v>
@@ -4445,7 +4445,7 @@
         <v>75</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F32" s="23">
         <v>1</v>

</xml_diff>

<commit_message>
add Contrasts sheet to excel template
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_template.xlsx
+++ b/inst/extdata/scidb_metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/reveal-genomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E81F64-4DEC-184F-85CB-5CD76AABEE59}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF7FF90-C223-EC40-ADDB-B009A69269B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="30160" windowHeight="17700" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="filter_choices" sheetId="7" r:id="rId6"/>
     <sheet name="featureset_choices" sheetId="8" r:id="rId7"/>
     <sheet name="Definitions" sheetId="3" r:id="rId8"/>
+    <sheet name="Contrasts" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Pipelines!$A$1:$L$4</definedName>
@@ -3443,7 +3444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+    <sheetView zoomScale="61" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
@@ -4601,4 +4602,16 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFD03B9-6AEB-894E-9EA0-0B688ECB9058}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated Definitions sheet of Excel sheet
- added columns for "attribute_in_pipeline_choices", "attribute_in_filter_choices", "attribute_in_featureset_choices"
- added attributes from the respective Sheets as rows in Definitions attribute
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_template.xlsx
+++ b/inst/extdata/scidb_metadata_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/reveal-genomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF7FF90-C223-EC40-ADDB-B009A69269B9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C03FA0-A448-7E4C-922F-3496F395F413}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="158">
   <si>
     <t>project_id</t>
   </si>
@@ -587,13 +587,22 @@
   </si>
   <si>
     <t>attribute_found_in_any_sheet</t>
+  </si>
+  <si>
+    <t>attribute_in_pipeline_choices</t>
+  </si>
+  <si>
+    <t>attribute_in_filter_choices</t>
+  </si>
+  <si>
+    <t>attribute_in_featureset_choices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -716,6 +725,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -791,7 +806,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -833,11 +848,92 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color theme="9" tint="0.79998168889431442"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="0.79998168889431442"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="0.79998168889431442"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="0.79998168889431442"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="0.79998168889431442"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -3442,11 +3538,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView zoomScale="61" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18"/>
@@ -3461,7 +3557,7 @@
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="161">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="171">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
@@ -3495,8 +3591,17 @@
       <c r="K1" s="22" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L1" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
@@ -3507,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="23" t="b">
-        <f>IF(COUNTIF(H2:K2,"TRUE")&gt;0,TRUE,FALSE)</f>
+        <f t="shared" ref="G2:G50" si="0">IF(COUNTIF(H2:N2,"TRUE")&gt;0,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H2" s="23" t="b">
@@ -3526,8 +3631,20 @@
         <f>IF(ISERROR(MATCH($A2,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L2" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A2,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M2" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A2,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N2" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A2,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A3" s="23" t="s">
         <v>3</v>
       </c>
@@ -3538,7 +3655,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="23" t="b">
-        <f t="shared" ref="G3:G32" si="0">IF(COUNTIF(H3:K3,"TRUE")&gt;0,TRUE,FALSE)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H3" s="23" t="b">
@@ -3557,8 +3674,20 @@
         <f>IF(ISERROR(MATCH($A3,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L3" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A3,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M3" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A3,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N3" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A3,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A4" s="23" t="s">
         <v>5</v>
       </c>
@@ -3588,8 +3717,20 @@
         <f>IF(ISERROR(MATCH($A4,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L4" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A4,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M4" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A4,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N4" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A4,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A5" s="23" t="s">
         <v>1</v>
       </c>
@@ -3619,8 +3760,20 @@
         <f>IF(ISERROR(MATCH($A5,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L5" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A5,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M5" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A5,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N5" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A5,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A6" s="23" t="s">
         <v>2</v>
       </c>
@@ -3650,8 +3803,20 @@
         <f>IF(ISERROR(MATCH($A6,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L6" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A6,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M6" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A6,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N6" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A6,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
@@ -3681,8 +3846,20 @@
         <f>IF(ISERROR(MATCH($A7,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L7" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A7,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M7" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A7,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N7" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A7,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A8" s="23" t="s">
         <v>6</v>
       </c>
@@ -3712,8 +3889,20 @@
         <f>IF(ISERROR(MATCH($A8,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L8" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A8,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M8" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A8,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N8" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A8,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A9" s="23" t="s">
         <v>7</v>
       </c>
@@ -3746,8 +3935,20 @@
         <f>IF(ISERROR(MATCH($A9,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L9" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A9,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M9" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A9,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N9" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A9,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
@@ -3777,8 +3978,20 @@
         <f>IF(ISERROR(MATCH($A10,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L10" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A10,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M10" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A10,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N10" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A10,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A11" s="23" t="s">
         <v>9</v>
       </c>
@@ -3808,8 +4021,20 @@
         <f>IF(ISERROR(MATCH($A11,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L11" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A11,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M11" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A11,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N11" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A11,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A12" s="23" t="s">
         <v>10</v>
       </c>
@@ -3839,8 +4064,20 @@
         <f>IF(ISERROR(MATCH($A12,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L12" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A12,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M12" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A12,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N12" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A12,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A13" s="23" t="s">
         <v>11</v>
       </c>
@@ -3870,8 +4107,20 @@
         <f>IF(ISERROR(MATCH($A13,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L13" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A13,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M13" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A13,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N13" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A13,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A14" s="23" t="s">
         <v>12</v>
       </c>
@@ -3904,8 +4153,20 @@
         <f>IF(ISERROR(MATCH($A14,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L14" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A14,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M14" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A14,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N14" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A14,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A15" s="23" t="s">
         <v>13</v>
       </c>
@@ -3935,8 +4196,20 @@
         <f>IF(ISERROR(MATCH($A15,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L15" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A15,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M15" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A15,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N15" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A15,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A16" s="23" t="s">
         <v>14</v>
       </c>
@@ -3966,8 +4239,20 @@
         <f>IF(ISERROR(MATCH($A16,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L16" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A16,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M16" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A16,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N16" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A16,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A17" s="23" t="s">
         <v>15</v>
       </c>
@@ -3997,8 +4282,20 @@
         <f>IF(ISERROR(MATCH($A17,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L17" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A17,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M17" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A17,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N17" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A17,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A18" s="23" t="s">
         <v>16</v>
       </c>
@@ -4028,8 +4325,20 @@
         <f>IF(ISERROR(MATCH($A18,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L18" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A18,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M18" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A18,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N18" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A18,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A19" s="23" t="s">
         <v>33</v>
       </c>
@@ -4059,8 +4368,20 @@
         <f>IF(ISERROR(MATCH($A19,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L19" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A19,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M19" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A19,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N19" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A19,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A20" s="23" t="s">
         <v>119</v>
       </c>
@@ -4093,8 +4414,20 @@
         <f>IF(ISERROR(MATCH($A20,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L20" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A20,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M20" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A20,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N20" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A20,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A21" s="23" t="s">
         <v>39</v>
       </c>
@@ -4124,8 +4457,20 @@
         <f>IF(ISERROR(MATCH($A21,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L21" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A21,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M21" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A21,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N21" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A21,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A22" s="23" t="s">
         <v>40</v>
       </c>
@@ -4155,8 +4500,20 @@
         <f>IF(ISERROR(MATCH($A22,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L22" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A22,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M22" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A22,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N22" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A22,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A23" s="23" t="s">
         <v>44</v>
       </c>
@@ -4189,8 +4546,20 @@
         <f>IF(ISERROR(MATCH($A23,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L23" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A23,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M23" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A23,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N23" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A23,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A24" s="23" t="s">
         <v>47</v>
       </c>
@@ -4220,8 +4589,20 @@
         <f>IF(ISERROR(MATCH($A24,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L24" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A24,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M24" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A24,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N24" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A24,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A25" s="23" t="s">
         <v>49</v>
       </c>
@@ -4254,8 +4635,20 @@
         <f>IF(ISERROR(MATCH($A25,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L25" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A25,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M25" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A25,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N25" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A25,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A26" s="23" t="s">
         <v>69</v>
       </c>
@@ -4285,8 +4678,20 @@
         <f>IF(ISERROR(MATCH($A26,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L26" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A26,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M26" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A26,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N26" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A26,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A27" s="23" t="s">
         <v>70</v>
       </c>
@@ -4316,8 +4721,20 @@
         <f>IF(ISERROR(MATCH($A27,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L27" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A27,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M27" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A27,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N27" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A27,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A28" s="23" t="s">
         <v>71</v>
       </c>
@@ -4347,8 +4764,20 @@
         <f>IF(ISERROR(MATCH($A28,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L28" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A28,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M28" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A28,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N28" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A28,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A29" s="23" t="s">
         <v>72</v>
       </c>
@@ -4378,8 +4807,20 @@
         <f>IF(ISERROR(MATCH($A29,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L29" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A29,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M29" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A29,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N29" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A29,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A30" s="23" t="s">
         <v>73</v>
       </c>
@@ -4409,8 +4850,20 @@
         <f>IF(ISERROR(MATCH($A30,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L30" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A30,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M30" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A30,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N30" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A30,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A31" s="23" t="s">
         <v>74</v>
       </c>
@@ -4440,8 +4893,20 @@
         <f>IF(ISERROR(MATCH($A31,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" s="23" customFormat="1" ht="19">
+      <c r="L31" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A31,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M31" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A31,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N31" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A31,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="23" customFormat="1" ht="19">
       <c r="A32" s="23" t="s">
         <v>75</v>
       </c>
@@ -4471,16 +4936,845 @@
         <f>IF(ISERROR(MATCH($A32,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v>1</v>
       </c>
+      <c r="L32" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A32,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M32" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A32,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N32" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A32,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="19">
+      <c r="A33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="23">
+        <v>1</v>
+      </c>
+      <c r="G33" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A33,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I33" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A33,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J33" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A33,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K33" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A33,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L33" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A33,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M33" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A33,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N33" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A33,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="19">
+      <c r="A34" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="23">
+        <v>1</v>
+      </c>
+      <c r="G34" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H34" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A34,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I34" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A34,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J34" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A34,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K34" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A34,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L34" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A34,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M34" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A34,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="N34" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A34,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="19">
+      <c r="A35" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="23">
+        <v>1</v>
+      </c>
+      <c r="G35" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H35" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A35,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I35" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A35,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J35" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A35,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K35" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A35,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L35" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A35,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M35" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A35,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N35" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A35,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="19">
+      <c r="A36" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="23">
+        <v>1</v>
+      </c>
+      <c r="G36" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H36" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A36,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I36" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A36,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J36" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A36,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K36" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A36,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L36" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A36,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M36" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A36,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N36" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A36,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="19">
+      <c r="A37" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="23">
+        <v>1</v>
+      </c>
+      <c r="G37" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H37" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A37,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I37" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A37,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J37" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A37,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K37" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A37,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L37" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A37,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M37" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A37,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N37" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A37,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="19">
+      <c r="A38" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="23">
+        <v>1</v>
+      </c>
+      <c r="G38" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H38" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A38,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I38" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A38,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J38" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A38,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K38" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A38,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L38" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A38,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M38" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A38,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N38" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A38,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="19">
+      <c r="A39" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="23">
+        <v>1</v>
+      </c>
+      <c r="G39" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H39" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A39,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I39" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A39,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J39" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A39,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K39" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A39,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L39" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A39,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M39" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A39,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N39" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A39,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="19">
+      <c r="A40" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="23">
+        <v>1</v>
+      </c>
+      <c r="G40" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H40" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A40,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I40" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A40,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J40" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A40,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K40" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A40,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L40" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A40,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M40" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A40,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N40" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A40,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="19">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="23">
+        <v>1</v>
+      </c>
+      <c r="G41" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H41" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A41,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I41" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A41,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J41" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A41,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K41" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A41,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L41" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A41,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M41" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A41,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="N41" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A41,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="19">
+      <c r="A42" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="23">
+        <v>1</v>
+      </c>
+      <c r="G42" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H42" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A42,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I42" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A42,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J42" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A42,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K42" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A42,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L42" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A42,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M42" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A42,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="N42" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A42,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="19">
+      <c r="A43" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="23">
+        <v>1</v>
+      </c>
+      <c r="G43" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H43" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A43,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I43" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A43,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J43" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A43,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K43" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A43,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L43" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A43,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M43" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A43,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="N43" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A43,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="19">
+      <c r="A44" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F44" s="23">
+        <v>1</v>
+      </c>
+      <c r="G44" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H44" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A44,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I44" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A44,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J44" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A44,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K44" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A44,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L44" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A44,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M44" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A44,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="N44" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A44,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="19">
+      <c r="A45" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" s="23">
+        <v>1</v>
+      </c>
+      <c r="G45" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H45" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A45,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I45" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A45,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J45" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A45,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K45" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A45,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L45" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A45,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="M45" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A45,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+      <c r="N45" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A45,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="19">
+      <c r="A46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F46" s="23">
+        <v>1</v>
+      </c>
+      <c r="G46" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H46" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A46,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I46" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A46,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J46" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A46,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K46" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A46,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L46" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A46,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M46" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A46,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N46" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A46,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="19">
+      <c r="A47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" s="23">
+        <v>1</v>
+      </c>
+      <c r="G47" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H47" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A47,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I47" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A47,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J47" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A47,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K47" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A47,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L47" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A47,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M47" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A47,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N47" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A47,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="19">
+      <c r="A48" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F48" s="23">
+        <v>1</v>
+      </c>
+      <c r="G48" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H48" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A48,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I48" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A48,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J48" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A48,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K48" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A48,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L48" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A48,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M48" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A48,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N48" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A48,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="19">
+      <c r="A49" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F49" s="23">
+        <v>1</v>
+      </c>
+      <c r="G49" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H49" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A49,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I49" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A49,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J49" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A49,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K49" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A49,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L49" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A49,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M49" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A49,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N49" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A49,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="19">
+      <c r="A50" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F50" s="23">
+        <v>1</v>
+      </c>
+      <c r="G50" s="23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H50" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A50,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I50" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A50,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J50" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A50,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K50" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A50,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L50" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A50,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M50" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A50,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N50" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A50,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="19">
+      <c r="A51" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F51" s="23">
+        <v>1</v>
+      </c>
+      <c r="G51" s="23" t="b">
+        <f>IF(COUNTIF(H51:N51,"TRUE")&gt;0,TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H51" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A51,Studies!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="I51" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A51,Subjects!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="J51" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A51,Samples!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="K51" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A51,Pipelines!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="L51" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A51,pipeline_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="M51" s="23" t="str">
+        <f>IF(ISERROR(MATCH($A51,filter_choices!$1:$1,0)),"",TRUE)</f>
+        <v/>
+      </c>
+      <c r="N51" s="23" t="b">
+        <f>IF(ISERROR(MATCH($A51,featureset_choices!$1:$1,0)),"",TRUE)</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="18" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H19)))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4494,18 +5788,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:K2 H4:K32">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="12">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4519,18 +5813,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:K4">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H18 H2">
-    <cfRule type="cellIs" dxfId="5" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="29" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="21" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="30" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4544,19 +5838,67 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G32">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33:H51">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",H33)))</formula>
+    </cfRule>
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9D993EE4-125A-8749-8C1F-721EAE556EF8}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33:K51">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G51">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L51">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G32">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="M2:M51">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>1</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N51">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4598,6 +5940,17 @@
           </x14:cfRule>
           <xm:sqref>H4:H18 H2</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9D993EE4-125A-8749-8C1F-721EAE556EF8}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H33:H51</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -4608,7 +5961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFD03B9-6AEB-894E-9EA0-0B688ECB9058}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>

</xml_diff>

<commit_message>
fix #39 (duplicate Definition of measurement_entity)
- also some minor font changes in Excel sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/scidb_metadata_template.xlsx
+++ b/inst/extdata/scidb_metadata_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kritisensharma/coding/downloads/reveal-genomics/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C03FA0-A448-7E4C-922F-3496F395F413}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430C7910-E01A-DF43-9F3E-5EC42B018C90}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="158">
   <si>
     <t>project_id</t>
   </si>
@@ -602,7 +602,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -725,12 +725,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -806,7 +800,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -848,72 +842,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color theme="9" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2877,17 +2810,17 @@
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000002000000}">
+          <x14:formula1>
+            <xm:f>featureset_choices!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>pipeline_choices!A$2:A$10</xm:f>
           </x14:formula1>
           <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000002000000}">
-          <x14:formula1>
-            <xm:f>featureset_choices!$A$2:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3538,11 +3471,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18"/>
@@ -3612,7 +3545,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="23" t="b">
-        <f t="shared" ref="G2:G50" si="0">IF(COUNTIF(H2:N2,"TRUE")&gt;0,TRUE,FALSE)</f>
+        <f t="shared" ref="G2:G49" si="0">IF(COUNTIF(H2:N2,"TRUE")&gt;0,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H2" s="23" t="b">
@@ -4950,7 +4883,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="19">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="23" t="s">
         <v>50</v>
       </c>
       <c r="B33" s="6" t="s">
@@ -4993,7 +4926,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="19">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="23" t="s">
         <v>51</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -5036,7 +4969,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="19">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B35" s="6" t="s">
@@ -5079,7 +5012,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" ht="19">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="23" t="s">
         <v>53</v>
       </c>
       <c r="B36" s="6" t="s">
@@ -5122,7 +5055,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" ht="19">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="23" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -5165,7 +5098,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" ht="19">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="23" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="6" t="s">
@@ -5208,7 +5141,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="19">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="23" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -5251,7 +5184,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" ht="19">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -5294,7 +5227,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="19">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="23" t="s">
         <v>85</v>
       </c>
       <c r="B41" s="6" t="s">
@@ -5337,7 +5270,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="19">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="23" t="s">
         <v>86</v>
       </c>
       <c r="B42" s="6" t="s">
@@ -5380,7 +5313,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="19">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="23" t="s">
         <v>87</v>
       </c>
       <c r="B43" s="6" t="s">
@@ -5423,7 +5356,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="19">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B44" s="6" t="s">
@@ -5466,8 +5399,8 @@
       </c>
     </row>
     <row r="45" spans="1:14" ht="19">
-      <c r="A45" s="29" t="s">
-        <v>51</v>
+      <c r="A45" s="23" t="s">
+        <v>134</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>115</v>
@@ -5495,22 +5428,22 @@
         <f>IF(ISERROR(MATCH($A45,Pipelines!$1:$1,0)),"",TRUE)</f>
         <v/>
       </c>
-      <c r="L45" s="23" t="b">
+      <c r="L45" s="23" t="str">
         <f>IF(ISERROR(MATCH($A45,pipeline_choices!$1:$1,0)),"",TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="M45" s="23" t="b">
+        <v/>
+      </c>
+      <c r="M45" s="23" t="str">
         <f>IF(ISERROR(MATCH($A45,filter_choices!$1:$1,0)),"",TRUE)</f>
-        <v>1</v>
-      </c>
-      <c r="N45" s="23" t="str">
+        <v/>
+      </c>
+      <c r="N45" s="23" t="b">
         <f>IF(ISERROR(MATCH($A45,featureset_choices!$1:$1,0)),"",TRUE)</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="19">
-      <c r="A46" s="1" t="s">
-        <v>134</v>
+      <c r="A46" s="23" t="s">
+        <v>135</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>115</v>
@@ -5552,8 +5485,8 @@
       </c>
     </row>
     <row r="47" spans="1:14" ht="19">
-      <c r="A47" s="1" t="s">
-        <v>135</v>
+      <c r="A47" s="23" t="s">
+        <v>136</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>115</v>
@@ -5595,8 +5528,8 @@
       </c>
     </row>
     <row r="48" spans="1:14" ht="19">
-      <c r="A48" s="29" t="s">
-        <v>136</v>
+      <c r="A48" s="23" t="s">
+        <v>137</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>115</v>
@@ -5638,8 +5571,8 @@
       </c>
     </row>
     <row r="49" spans="1:14" ht="19">
-      <c r="A49" s="29" t="s">
-        <v>137</v>
+      <c r="A49" s="23" t="s">
+        <v>138</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>115</v>
@@ -5681,8 +5614,8 @@
       </c>
     </row>
     <row r="50" spans="1:14" ht="19">
-      <c r="A50" s="29" t="s">
-        <v>138</v>
+      <c r="A50" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>115</v>
@@ -5691,7 +5624,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="23" t="b">
-        <f t="shared" si="0"/>
+        <f>IF(COUNTIF(H50:N50,"TRUE")&gt;0,TRUE,FALSE)</f>
         <v>1</v>
       </c>
       <c r="H50" s="23" t="str">
@@ -5723,55 +5656,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="19">
-      <c r="A51" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F51" s="23">
-        <v>1</v>
-      </c>
-      <c r="G51" s="23" t="b">
-        <f>IF(COUNTIF(H51:N51,"TRUE")&gt;0,TRUE,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="H51" s="23" t="str">
-        <f>IF(ISERROR(MATCH($A51,Studies!$1:$1,0)),"",TRUE)</f>
-        <v/>
-      </c>
-      <c r="I51" s="23" t="str">
-        <f>IF(ISERROR(MATCH($A51,Subjects!$1:$1,0)),"",TRUE)</f>
-        <v/>
-      </c>
-      <c r="J51" s="23" t="str">
-        <f>IF(ISERROR(MATCH($A51,Samples!$1:$1,0)),"",TRUE)</f>
-        <v/>
-      </c>
-      <c r="K51" s="23" t="str">
-        <f>IF(ISERROR(MATCH($A51,Pipelines!$1:$1,0)),"",TRUE)</f>
-        <v/>
-      </c>
-      <c r="L51" s="23" t="str">
-        <f>IF(ISERROR(MATCH($A51,pipeline_choices!$1:$1,0)),"",TRUE)</f>
-        <v/>
-      </c>
-      <c r="M51" s="23" t="str">
-        <f>IF(ISERROR(MATCH($A51,filter_choices!$1:$1,0)),"",TRUE)</f>
-        <v/>
-      </c>
-      <c r="N51" s="23" t="b">
-        <f>IF(ISERROR(MATCH($A51,featureset_choices!$1:$1,0)),"",TRUE)</f>
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="H19:H32">
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="26" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="27" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="27" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H19)))</formula>
     </cfRule>
     <cfRule type="dataBar" priority="28">
@@ -5787,16 +5677,16 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:K2 H4:K32">
-    <cfRule type="cellIs" dxfId="17" priority="22" operator="equal">
+  <conditionalFormatting sqref="H2:K2 H4:K50 L2:N50">
+    <cfRule type="cellIs" dxfId="11" priority="22" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="20" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H3)))</formula>
     </cfRule>
     <cfRule type="dataBar" priority="21">
@@ -5813,15 +5703,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:K4">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H18 H2">
-    <cfRule type="cellIs" dxfId="13" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="29" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="30" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="30" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H2)))</formula>
     </cfRule>
     <cfRule type="dataBar" priority="31">
@@ -5837,30 +5727,30 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+  <conditionalFormatting sqref="G2:G50">
+    <cfRule type="cellIs" dxfId="5" priority="12" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="15" operator="equal">
       <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G32">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H33:H51">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+  <conditionalFormatting sqref="H33:H50">
+    <cfRule type="cellIs" dxfId="1" priority="32" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="33" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",H33)))</formula>
     </cfRule>
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="34">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5871,34 +5761,6 @@
           <x14:id>{9D993EE4-125A-8749-8C1F-721EAE556EF8}</x14:id>
         </ext>
       </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H33:K51">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G51">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L51">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M51">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N51">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5949,7 +5811,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H33:H51</xm:sqref>
+          <xm:sqref>H33:H50</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>